<commit_message>
add dropdown select profile, datepicker for double click pop up
</commit_message>
<xml_diff>
--- a/upload_data.xlsx
+++ b/upload_data.xlsx
@@ -466,32 +466,22 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>E:\storage\128G.mp4</t>
+          <t>E:\storage\75G.mp4</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>ád</t>
+          <t>áda</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>ád</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>10/02/2025</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>17:52</t>
+          <t>ádas</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>E:/New folder\128G.mp4</t>
+          <t>E:/New folder\75G.mp4</t>
         </is>
       </c>
     </row>

</xml_diff>